<commit_message>
Fix wrong description for 74HC04.
</commit_message>
<xml_diff>
--- a/Modules/kNOT/kNOT_BOM.xlsx
+++ b/Modules/kNOT/kNOT_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\kNOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81BA2F2-E61F-44D0-9D92-B63B4F20D1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6473D08-CCF9-4596-8534-BBBA4291436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>DIP-14</t>
   </si>
   <si>
-    <t>Quad AND 2 inputs</t>
-  </si>
-  <si>
     <t>Quad Op Amp</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
+  </si>
+  <si>
+    <t>Hex Inverter</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1195,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -1237,16 +1237,16 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1257,16 +1257,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1277,16 +1277,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,16 +1297,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1317,16 +1317,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,16 +1337,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,16 +1357,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1377,16 +1377,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1394,19 +1394,19 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,13 +1420,13 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1434,19 +1434,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1457,16 +1457,16 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1480,13 +1480,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1494,19 +1494,19 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1514,19 +1514,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1534,19 +1534,19 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,19 +1554,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1574,19 +1574,19 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,16 +1594,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,16 +1611,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1628,16 +1628,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,16 +1645,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,16 +1662,16 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,16 +1679,16 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>